<commit_message>
Code after revision 1
</commit_message>
<xml_diff>
--- a/Visuals/Tables/Supplementary Table 1.xlsx
+++ b/Visuals/Tables/Supplementary Table 1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,98 +436,1573 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Change in Mean (%)</t>
+          <t>Mean Annual BA 2001-2020 GFED5 (Mha)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>Mean Change CC (%)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>KS Statistic</t>
+          <t>Mean Change DHF (%)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mean Change All (%)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>PR due to climate change</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>1980-2019 Overburning trend</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>1901-1920</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4742554854601622</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.021544254508889</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.01605999999999996</v>
+        <v>783.0666458686643</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>17.3 [14.1, 21.1]</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-21.1 [-23.9, -17.8]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-7.0 [-9.4, -4.3]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1.25 [1.2, 1.3]</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.23 [0.22, 0.26]</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>1950-2019</t>
+          <t>ARP</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9.460000693798065</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.27019644691126</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.13118</v>
+        <v>0.04457282502310986</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10.7 [-3.9, 30.0]</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-8.2 [-24.3, 2.8]</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>10.9 [-4.2, 30.0]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1.04 [0.99, 1.09]</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.5 [-0.27, 1.49]</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2003-2019</t>
+          <t>CAF</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>16.42533987760544</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.425367255201817</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.18993</v>
+        <v>150.0442123779138</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>21.1 [16.8, 26.2]</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-15.8 [-20.2, -11.4]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1.5 [-3.8, 6.7]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1.17 [1.13, 1.21]</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.35 [0.34, 0.36]</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>DHF</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-15.82963764667511</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.4726257461329454</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.34753</v>
+        <v>1.159821136108151</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-6.3 [-11.2, -1.5]</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>-33.3 [-42.4, -25.7]</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-35.5 [-44.5, -27.7]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.95 [0.91, 0.99]</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-0.1 [-0.14, -0.05]</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>All Forcing</t>
+          <t>CAU</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-3.715059533715248</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.8403328983119746</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.16545</v>
+        <v>10.55604622111864</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>86.6 [62.5, 121.3]</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-10.0 [-17.9, -3.5]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>60.5 [42.8, 88.5]</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1.32 [1.25, 1.39]</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>4.79 [3.93, 5.84]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>CNA</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3.204786850525409</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>7.6 [3.4, 12.0]</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>-3.0 [-9.8, 4.1]</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>3.7 [-4.2, 12.0]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1.05 [1.02, 1.07]</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.16 [0.11, 0.23]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>EAS</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>12.99786729482585</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.8 [-4.1, 7.5]</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-39.4 [-50.6, -30.1]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-38.7 [-49.9, -29.6]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1.01 [0.98, 1.04]</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-0.03 [-0.06, -0.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>EAU</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>5.142660335270539</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>31.4 [25.0, 40.4]</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2.3 [-4.3, 10.1]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>32.1 [22.1, 42.3]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1.17 [1.13, 1.22]</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.76 [0.68, 0.84]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>ECA</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.9132422913942072</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>24.6 [18.1, 32.6]</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>-6.4 [-14.3, 0.2]</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>16.2 [7.0, 24.4]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1.13 [1.09, 1.16]</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.54 [0.48, 0.62]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>EEU</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>11.09371655697392</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>9.9 [6.4, 14.8]</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>-3.5 [-8.8, 0.8]</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>9.1 [3.0, 16.7]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1.09 [1.05, 1.12]</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1.15 [0.81, 1.61]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1.324710730240897</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>7.1 [1.7, 14.6]</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>-26.5 [-35.4, -19.0]</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-22.5 [-29.4, -15.7]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1.05 [1.01, 1.1]</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.05 [-0.05, 0.21]</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>ESAF</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>77.76832868239563</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>7.1 [2.1, 12.3]</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>-7.6 [-13.7, -1.6]</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-1.1 [-7.3, 5.0]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>1.04 [1.01, 1.08]</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0.14 [0.14, 0.15]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>ESB</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>15.61116855315357</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>12.2 [6.6, 19.9]</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>-8.4 [-16.6, -1.2]</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2.6 [-6.2, 11.5]</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>1.09 [1.04, 1.15]</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.24 [0.17, 0.31]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>MDG</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>14.18143281800756</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>6.3 [1.0, 12.7]</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>12.0 [3.7, 20.2]</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>17.1 [8.6, 26.0]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1.04 [1.01, 1.07]</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.19 [0.17, 0.21]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>MED</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.571690681562189</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>13.9 [10.3, 17.7]</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>-9.8 [-13.2, -6.2]</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-0.0 [-3.7, 4.5]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>1.1 [1.07, 1.13]</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.47 [0.45, 0.48]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>NAU</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>40.12907389128333</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>15.2 [10.2, 21.2]</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>37.5 [28.8, 47.7]</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>59.4 [49.1, 71.1]</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>1.1 [1.07, 1.14]</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.48 [0.39, 0.58]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>NCA</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.267386909601271</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>23.8 [17.3, 31.6]</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>-19.2 [-26.9, -12.1]</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-2.6 [-9.8, 5.3]</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>1.14 [1.1, 1.19]</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0.45 [0.38, 0.51]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>NEAF</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>65.28164824631922</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>10.6 [6.2, 15.4]</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>-18.2 [-23.8, -13.3]</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-10.1 [-15.1, -5.3]</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>1.07 [1.04, 1.11]</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0.22 [0.18, 0.25]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>NEN</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1.257057078607712</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.3 [-1.8, 2.6]</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>-9.2 [-14.6, -5.6]</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-9.1 [-14.7, -5.6]</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>1.0 [0.98, 1.03]</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-0.08 [-0.18, 0.07]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>NES</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>16.40368162342518</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>-17.8 [-24.7, -11.7]</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>-24.9 [-34.1, -17.6]</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-37.1 [-47.3, -28.8]</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0.88 [0.85, 0.92]</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-0.04 [-0.07, -0.01]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>NEU</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.4708144071059426</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>12.2 [6.1, 21.2]</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>-9.8 [-17.6, -2.6]</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.2 [-7.9, 9.2]</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>1.06 [1.04, 1.1]</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0.77 [0.6, 0.97]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>NSA</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>10.08959778482704</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-3.9 [-8.4, 0.1]</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>3.6 [-3.5, 11.3]</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-1.3 [-8.6, 5.7]</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>0.97 [0.94, 1.0]</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0.16 [0.13, 0.2]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>NWN</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2.472289377306868</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1.4 [-0.2, 3.0]</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>-13.1 [-18.5, -8.9]</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-12.1 [-17.6, -7.8]</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>1.03 [1.0, 1.05]</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-0.09 [-0.16, -0.03]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>NWS</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>3.098759226388636</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>16.6 [8.6, 25.3]</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>-17.9 [-27.1, -9.6]</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>-4.0 [-12.9, 4.1]</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>1.09 [1.05, 1.14]</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0.15 [0.07, 0.24]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>NZ</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.0328581571668209</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2.8 [0.4, 6.1]</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>7.8 [2.9, 14.5]</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>12.3 [5.6, 19.8]</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>1.02 [1.0, 1.05]</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>0.13 [0.0, 0.26]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>RAR</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1.488307596582129</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>-0.8 [-2.5, 0.8]</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>-19.4 [-30.4, -11.2]</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-20.0 [-31.2, -11.4]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>0.98 [0.95, 1.02]</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-0.15 [-0.29, -0.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>RFE</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>5.470477053823565</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-2.3 [-7.0, 2.1]</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>-9.8 [-15.7, -4.2]</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-11.7 [-18.1, -5.4]</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>0.98 [0.94, 1.02]</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-0.34 [-0.44, -0.19]</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>SAH</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2.63523842569335</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>16.3 [9.4, 23.1]</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>11.3 [1.3, 19.9]</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>29.5 [18.8, 41.1]</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>1.09 [1.05, 1.13]</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0.18 [0.15, 0.21]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>SAM</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>16.42524269919482</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>4.2 [0.3, 8.3]</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>-17.0 [-23.6, -11.3]</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>-13.5 [-20.2, -7.2]</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>1.04 [1.0, 1.07]</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0.35 [0.3, 0.39]</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>23.81595256411641</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2.2 [-0.6, 5.4]</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>-17.9 [-23.0, -13.7]</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>-17.0 [-21.8, -12.9]</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>1.03 [0.99, 1.08]</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-0.02 [-0.04, 0.01]</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>SAU</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2.720063890960294</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>19.0 [13.8, 25.3]</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>-7.6 [-14.0, -2.1]</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>7.1 [-0.6, 14.9]</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>1.1 [1.07, 1.14]</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>0.45 [0.4, 0.59]</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>SCA</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>8.059580624577196</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>4.2 [-0.4, 8.5]</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>-24.1 [-30.6, -18.6]</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>-21.7 [-27.9, -16.1]</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>1.04 [1.0, 1.07]</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>0.44 [0.39, 0.47]</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>SEA</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>27.82945029199584</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>-22.3 [-28.1, -17.2]</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>-49.3 [-57.6, -42.9]</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>-57.3 [-66.0, -50.2]</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>0.83 [0.78, 0.86]</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-0.34 [-0.35, -0.32]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>SEAF</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>40.28264284425475</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>4.6 [0.1, 9.1]</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>-24.5 [-30.4, -19.3]</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>-21.0 [-27.4, -14.8]</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>1.04 [1.0, 1.07]</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>0.08 [0.07, 0.08]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>SES</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>15.80127240386313</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>17.9 [12.7, 23.9]</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>-25.9 [-31.1, -21.2]</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-14.5 [-19.7, -9.6]</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>1.15 [1.1, 1.19]</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>0.52 [0.45, 0.59]</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>SSA</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.1164706991914536</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>38.3 [25.3, 61.7]</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>6.5 [0.4, 15.5]</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>52.6 [33.6, 79.9]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>1.16 [1.12, 1.21]</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2.27 [1.85, 2.71]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>SWS</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.8675885220775453</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>32.4 [23.8, 44.7]</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2.7 [-4.7, 10.7]</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>38.2 [27.5, 53.3]</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>1.14 [1.11, 1.19]</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>1.14 [0.9, 1.31]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>TIB</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>3.554047520629116</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>98.5 [74.6, 130.6]</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>-49.9 [-63.2, -39.3]</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-23.5 [-35.1, -13.8]</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>1.36 [1.29, 1.43]</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>4.04 [3.38, 4.82]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>WAF</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>98.27688410489203</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>7.4 [2.6, 12.6]</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>-24.0 [-29.5, -19.2]</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-20.3 [-25.9, -14.9]</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>1.05 [1.02, 1.08]</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>0.24 [0.2, 0.27]</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>WCA</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>6.577510871647408</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>31.2 [25.2, 39.8]</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>-12.5 [-17.9, -3.6]</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>13.4 [5.3, 33.1]</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>1.18 [1.14, 1.22]</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>0.81 [0.75, 0.9]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>WCE</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>9.899436049926996</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>6.4 [2.5, 10.8]</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2.4 [-5.3, 9.8]</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>8.6 [1.2, 17.8]</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>1.05 [1.02, 1.09]</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>0.17 [0.06, 0.28]</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>WNA</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1.817594141781888</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>13.2 [10.6, 16.5]</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>5.1 [1.4, 8.8]</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>19.1 [14.4, 24.9]</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>1.11 [1.08, 1.14]</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>0.53 [0.49, 0.56]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>WSAF</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>46.95443515924921</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>8.7 [4.5, 13.1]</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>5.0 [-2.1, 12.5]</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>15.4 [8.4, 23.3]</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>1.06 [1.03, 1.09]</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>0.1 [0.09, 0.1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>WSB</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>18.35702634766161</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>14.0 [9.3, 21.0]</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>-2.7 [-8.2, 2.0]</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>9.7 [3.5, 16.8]</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>1.11 [1.07, 1.15]</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>0.68 [0.62, 0.76]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating files after Revision 4
</commit_message>
<xml_diff>
--- a/Visuals/Tables/Supplementary Table 1.xlsx
+++ b/Visuals/Tables/Supplementary Table 1.xlsx
@@ -476,27 +476,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>17.3 [14.1, 21.1]</t>
+          <t>15.8 [13.1, 18.7]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-21.1 [-23.9, -17.8]</t>
+          <t>-19.1 [-21.9, -15.8]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-7.0 [-9.4, -4.3]</t>
+          <t>-5.0 [-7.6, -2.3]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.25 [1.2, 1.3]</t>
+          <t>1.22 [1.18, 1.26]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.23 [0.22, 0.26]</t>
+          <t>0.22 [0.22, 0.24]</t>
         </is>
       </c>
     </row>
@@ -511,27 +511,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10.7 [-3.9, 30.0]</t>
+          <t>-1.3 [-9.2, 7.6]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>-8.2 [-24.3, 2.8]</t>
+          <t>-9.3 [-17.4, -4.0]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10.9 [-4.2, 30.0]</t>
+          <t>2.4 [-5.7, 9.8]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.04 [0.99, 1.09]</t>
+          <t>0.99 [0.96, 1.04]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.5 [-0.27, 1.49]</t>
+          <t>0.43 [-0.08, 1.18]</t>
         </is>
       </c>
     </row>
@@ -546,27 +546,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>21.1 [16.8, 26.2]</t>
+          <t>20.3 [16.4, 24.7]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-15.8 [-20.2, -11.4]</t>
+          <t>-14.2 [-19.1, -9.2]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.5 [-3.8, 6.7]</t>
+          <t>3.2 [-2.0, 8.7]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1.17 [1.13, 1.21]</t>
+          <t>1.14 [1.11, 1.18]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.35 [0.34, 0.36]</t>
+          <t>0.31 [0.29, 0.34]</t>
         </is>
       </c>
     </row>
@@ -581,27 +581,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-6.3 [-11.2, -1.5]</t>
+          <t>-7.2 [-12.1, -2.5]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-33.3 [-42.4, -25.7]</t>
+          <t>-36.8 [-44.2, -31.0]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-35.5 [-44.5, -27.7]</t>
+          <t>-39.2 [-46.3, -33.3]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.95 [0.91, 0.99]</t>
+          <t>0.95 [0.92, 0.98]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-0.1 [-0.14, -0.05]</t>
+          <t>-0.06 [-0.1, -0.01]</t>
         </is>
       </c>
     </row>
@@ -616,27 +616,27 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>86.6 [62.5, 121.3]</t>
+          <t>61.9 [50.0, 78.7]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-10.0 [-17.9, -3.5]</t>
+          <t>-8.4 [-13.8, -3.3]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>60.5 [42.8, 88.5]</t>
+          <t>46.9 [37.3, 60.1]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1.32 [1.25, 1.39]</t>
+          <t>1.33 [1.28, 1.4]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>4.79 [3.93, 5.84]</t>
+          <t>3.04 [2.36, 3.9]</t>
         </is>
       </c>
     </row>
@@ -651,27 +651,27 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7.6 [3.4, 12.0]</t>
+          <t>8.1 [4.5, 11.7]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>-3.0 [-9.8, 4.1]</t>
+          <t>-1.2 [-7.2, 4.5]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3.7 [-4.2, 12.0]</t>
+          <t>5.8 [-0.2, 11.8]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1.05 [1.02, 1.07]</t>
+          <t>1.06 [1.03, 1.08]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.16 [0.11, 0.23]</t>
+          <t>0.19 [0.15, 0.23]</t>
         </is>
       </c>
     </row>
@@ -686,27 +686,27 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.8 [-4.1, 7.5]</t>
+          <t>0.8 [-3.5, 5.0]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-39.4 [-50.6, -30.1]</t>
+          <t>-38.1 [-46.1, -31.8]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-38.7 [-49.9, -29.6]</t>
+          <t>-37.6 [-45.8, -31.1]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1.01 [0.98, 1.04]</t>
+          <t>1.01 [0.98, 1.03]</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-0.03 [-0.06, -0.0]</t>
+          <t>-0.01 [-0.04, 0.03]</t>
         </is>
       </c>
     </row>
@@ -721,27 +721,27 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>31.4 [25.0, 40.4]</t>
+          <t>27.7 [22.8, 33.9]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2.3 [-4.3, 10.1]</t>
+          <t>2.3 [-3.4, 8.2]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>32.1 [22.1, 42.3]</t>
+          <t>27.8 [19.8, 35.8]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1.17 [1.13, 1.22]</t>
+          <t>1.18 [1.14, 1.21]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.76 [0.68, 0.84]</t>
+          <t>0.71 [0.64, 0.77]</t>
         </is>
       </c>
     </row>
@@ -756,27 +756,27 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>24.6 [18.1, 32.6]</t>
+          <t>27.7 [22.4, 34.4]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>-6.4 [-14.3, 0.2]</t>
+          <t>-4.4 [-10.3, 1.0]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>16.2 [7.0, 24.4]</t>
+          <t>21.1 [13.9, 28.3]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1.13 [1.09, 1.16]</t>
+          <t>1.14 [1.11, 1.17]</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.54 [0.48, 0.62]</t>
+          <t>0.56 [0.5, 0.62]</t>
         </is>
       </c>
     </row>
@@ -791,27 +791,27 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9.9 [6.4, 14.8]</t>
+          <t>12.3 [8.4, 17.1]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>-3.5 [-8.8, 0.8]</t>
+          <t>-2.4 [-7.3, 2.3]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>9.1 [3.0, 16.7]</t>
+          <t>12.5 [6.3, 20.7]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1.09 [1.05, 1.12]</t>
+          <t>1.08 [1.06, 1.11]</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>1.15 [0.81, 1.61]</t>
+          <t>1.16 [0.9, 1.43]</t>
         </is>
       </c>
     </row>
@@ -826,27 +826,27 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>7.1 [1.7, 14.6]</t>
+          <t>5.3 [1.1, 10.1]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>-26.5 [-35.4, -19.0]</t>
+          <t>-26.1 [-32.1, -20.0]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-22.5 [-29.4, -15.7]</t>
+          <t>-22.2 [-28.5, -16.3]</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>1.05 [1.01, 1.1]</t>
+          <t>1.04 [1.01, 1.08]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0.05 [-0.05, 0.21]</t>
+          <t>0.04 [-0.06, 0.15]</t>
         </is>
       </c>
     </row>
@@ -861,22 +861,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.1 [2.1, 12.3]</t>
+          <t>8.3 [3.6, 13.5]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>-7.6 [-13.7, -1.6]</t>
+          <t>-4.4 [-11.9, 2.4]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-1.1 [-7.3, 5.0]</t>
+          <t>4.0 [-3.7, 11.3]</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>1.04 [1.01, 1.08]</t>
+          <t>1.04 [1.02, 1.06]</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -896,27 +896,27 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>12.2 [6.6, 19.9]</t>
+          <t>11.3 [6.4, 16.9]</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>-8.4 [-16.6, -1.2]</t>
+          <t>-6.5 [-12.9, -1.5]</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2.6 [-6.2, 11.5]</t>
+          <t>3.4 [-2.5, 9.7]</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1.09 [1.04, 1.15]</t>
+          <t>1.08 [1.04, 1.12]</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0.24 [0.17, 0.31]</t>
+          <t>0.22 [0.16, 0.27]</t>
         </is>
       </c>
     </row>
@@ -931,27 +931,27 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6.3 [1.0, 12.7]</t>
+          <t>8.8 [3.1, 13.9]</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12.0 [3.7, 20.2]</t>
+          <t>17.4 [9.2, 25.1]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>17.1 [8.6, 26.0]</t>
+          <t>24.8 [15.2, 34.1]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>1.04 [1.01, 1.07]</t>
+          <t>1.04 [1.02, 1.07]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0.19 [0.17, 0.21]</t>
+          <t>0.21 [0.19, 0.22]</t>
         </is>
       </c>
     </row>
@@ -966,27 +966,27 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>13.9 [10.3, 17.7]</t>
+          <t>16.9 [12.7, 21.6]</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>-9.8 [-13.2, -6.2]</t>
+          <t>-11.2 [-16.5, -6.7]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>-0.0 [-3.7, 4.5]</t>
+          <t>1.1 [-4.2, 6.5]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>1.1 [1.07, 1.13]</t>
+          <t>1.09 [1.06, 1.11]</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0.47 [0.45, 0.48]</t>
+          <t>0.46 [0.45, 0.48]</t>
         </is>
       </c>
     </row>
@@ -1001,27 +1001,27 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>15.2 [10.2, 21.2]</t>
+          <t>22.4 [17.5, 27.7]</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>37.5 [28.8, 47.7]</t>
+          <t>32.4 [24.5, 42.8]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>59.4 [49.1, 71.1]</t>
+          <t>62.1 [51.1, 74.7]</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>1.1 [1.07, 1.14]</t>
+          <t>1.14 [1.11, 1.17]</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.48 [0.39, 0.58]</t>
+          <t>0.58 [0.52, 0.62]</t>
         </is>
       </c>
     </row>
@@ -1036,27 +1036,27 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>23.8 [17.3, 31.6]</t>
+          <t>23.6 [18.7, 29.2]</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>-19.2 [-26.9, -12.1]</t>
+          <t>-16.3 [-21.5, -11.4]</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>-2.6 [-9.8, 5.3]</t>
+          <t>1.5 [-4.8, 7.3]</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>1.14 [1.1, 1.19]</t>
+          <t>1.15 [1.12, 1.19]</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.45 [0.38, 0.51]</t>
+          <t>0.52 [0.46, 0.59]</t>
         </is>
       </c>
     </row>
@@ -1071,27 +1071,27 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10.6 [6.2, 15.4]</t>
+          <t>12.4 [6.3, 18.8]</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>-18.2 [-23.8, -13.3]</t>
+          <t>-21.5 [-28.9, -15.2]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>-10.1 [-15.1, -5.3]</t>
+          <t>-10.9 [-17.6, -4.9]</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>1.07 [1.04, 1.11]</t>
+          <t>1.06 [1.03, 1.09]</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0.22 [0.18, 0.25]</t>
+          <t>0.2 [0.17, 0.24]</t>
         </is>
       </c>
     </row>
@@ -1106,17 +1106,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.3 [-1.8, 2.6]</t>
+          <t>0.1 [-1.4, 1.5]</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>-9.2 [-14.6, -5.6]</t>
+          <t>-6.9 [-9.7, -4.8]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>-9.1 [-14.7, -5.6]</t>
+          <t>-6.8 [-9.7, -4.7]</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>-0.08 [-0.18, 0.07]</t>
+          <t>-0.01 [-0.24, 0.3]</t>
         </is>
       </c>
     </row>
@@ -1141,27 +1141,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>-17.8 [-24.7, -11.7]</t>
+          <t>-13.6 [-20.7, -7.3]</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>-24.9 [-34.1, -17.6]</t>
+          <t>-20.7 [-28.3, -13.8]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>-37.1 [-47.3, -28.8]</t>
+          <t>-30.0 [-38.8, -21.9]</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0.88 [0.85, 0.92]</t>
+          <t>0.93 [0.89, 0.96]</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>-0.04 [-0.07, -0.01]</t>
+          <t>-0.0 [-0.03, 0.05]</t>
         </is>
       </c>
     </row>
@@ -1176,27 +1176,27 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>12.2 [6.1, 21.2]</t>
+          <t>5.9 [3.0, 10.7]</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>-9.8 [-17.6, -2.6]</t>
+          <t>-9.1 [-13.4, -4.8]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.2 [-7.9, 9.2]</t>
+          <t>-3.6 [-8.2, 1.2]</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1.06 [1.04, 1.1]</t>
+          <t>1.05 [1.03, 1.08]</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0.77 [0.6, 0.97]</t>
+          <t>0.56 [0.38, 0.76]</t>
         </is>
       </c>
     </row>
@@ -1211,27 +1211,27 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>-3.9 [-8.4, 0.1]</t>
+          <t>-4.0 [-8.1, 0.2]</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3.6 [-3.5, 11.3]</t>
+          <t>5.3 [-1.8, 12.6]</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-1.3 [-8.6, 5.7]</t>
+          <t>0.6 [-6.4, 7.9]</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0.97 [0.94, 1.0]</t>
+          <t>0.98 [0.95, 1.0]</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0.16 [0.13, 0.2]</t>
+          <t>0.18 [0.14, 0.21]</t>
         </is>
       </c>
     </row>
@@ -1246,27 +1246,27 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.4 [-0.2, 3.0]</t>
+          <t>2.4 [0.6, 4.4]</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>-13.1 [-18.5, -8.9]</t>
+          <t>-10.1 [-13.8, -6.9]</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>-12.1 [-17.6, -7.8]</t>
+          <t>-8.6 [-12.3, -5.2]</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>1.03 [1.0, 1.05]</t>
+          <t>1.03 [1.01, 1.05]</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>-0.09 [-0.16, -0.03]</t>
+          <t>-0.05 [-0.12, 0.01]</t>
         </is>
       </c>
     </row>
@@ -1281,27 +1281,27 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>16.6 [8.6, 25.3]</t>
+          <t>9.5 [4.1, 16.6]</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>-17.9 [-27.1, -9.6]</t>
+          <t>-8.0 [-17.1, 0.5]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>-4.0 [-12.9, 4.1]</t>
+          <t>0.7 [-6.9, 8.0]</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>1.09 [1.05, 1.14]</t>
+          <t>1.06 [1.03, 1.09]</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>0.15 [0.07, 0.24]</t>
+          <t>0.09 [0.04, 0.16]</t>
         </is>
       </c>
     </row>
@@ -1316,27 +1316,27 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2.8 [0.4, 6.1]</t>
+          <t>3.1 [0.6, 6.4]</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>7.8 [2.9, 14.5]</t>
+          <t>9.8 [4.1, 16.3]</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>12.3 [5.6, 19.8]</t>
+          <t>14.7 [7.9, 22.7]</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>1.02 [1.0, 1.05]</t>
+          <t>1.03 [1.01, 1.05]</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>0.13 [0.0, 0.26]</t>
+          <t>0.13 [0.01, 0.25]</t>
         </is>
       </c>
     </row>
@@ -1351,27 +1351,27 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>-0.8 [-2.5, 0.8]</t>
+          <t>-0.1 [-0.6, 0.6]</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>-19.4 [-30.4, -11.2]</t>
+          <t>-14.9 [-21.2, -9.2]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>-20.0 [-31.2, -11.4]</t>
+          <t>-14.9 [-21.5, -9.1]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0.98 [0.95, 1.02]</t>
+          <t>1.0 [0.97, 1.02]</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>-0.15 [-0.29, -0.0]</t>
+          <t>0.08 [-0.14, 0.32]</t>
         </is>
       </c>
     </row>
@@ -1386,27 +1386,27 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>-2.3 [-7.0, 2.1]</t>
+          <t>-4.1 [-7.7, -0.7]</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>-9.8 [-15.7, -4.2]</t>
+          <t>-10.7 [-15.5, -5.9]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>-11.7 [-18.1, -5.4]</t>
+          <t>-14.0 [-19.0, -9.3]</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0.98 [0.94, 1.02]</t>
+          <t>0.97 [0.94, 0.99]</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>-0.34 [-0.44, -0.19]</t>
+          <t>-0.28 [-0.39, -0.18]</t>
         </is>
       </c>
     </row>
@@ -1421,27 +1421,27 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16.3 [9.4, 23.1]</t>
+          <t>16.1 [11.5, 21.0]</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>11.3 [1.3, 19.9]</t>
+          <t>10.7 [4.3, 17.6]</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>29.5 [18.8, 41.1]</t>
+          <t>27.9 [20.1, 37.8]</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>1.09 [1.05, 1.13]</t>
+          <t>1.1 [1.07, 1.13]</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0.18 [0.15, 0.21]</t>
+          <t>0.2 [0.17, 0.24]</t>
         </is>
       </c>
     </row>
@@ -1456,27 +1456,27 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>4.2 [0.3, 8.3]</t>
+          <t>3.4 [0.0, 6.8]</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>-17.0 [-23.6, -11.3]</t>
+          <t>-14.8 [-21.2, -9.7]</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>-13.5 [-20.2, -7.2]</t>
+          <t>-11.7 [-18.1, -5.8]</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>1.04 [1.0, 1.07]</t>
+          <t>1.02 [1.0, 1.05]</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>0.35 [0.3, 0.39]</t>
+          <t>0.29 [0.26, 0.32]</t>
         </is>
       </c>
     </row>
@@ -1491,27 +1491,27 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2.2 [-0.6, 5.4]</t>
+          <t>2.6 [-0.3, 5.8]</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>-17.9 [-23.0, -13.7]</t>
+          <t>-30.5 [-37.6, -24.7]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>-17.0 [-21.8, -12.9]</t>
+          <t>-29.4 [-36.2, -23.8]</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>1.03 [0.99, 1.08]</t>
+          <t>1.02 [1.0, 1.04]</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>-0.02 [-0.04, 0.01]</t>
+          <t>-0.02 [-0.03, 0.0]</t>
         </is>
       </c>
     </row>
@@ -1526,27 +1526,27 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>19.0 [13.8, 25.3]</t>
+          <t>20.0 [16.0, 24.9]</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>-7.6 [-14.0, -2.1]</t>
+          <t>-8.3 [-13.3, -3.7]</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>7.1 [-0.6, 14.9]</t>
+          <t>6.3 [1.0, 12.5]</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>1.1 [1.07, 1.14]</t>
+          <t>1.12 [1.09, 1.15]</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0.45 [0.4, 0.59]</t>
+          <t>0.55 [0.47, 0.61]</t>
         </is>
       </c>
     </row>
@@ -1561,27 +1561,27 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>4.2 [-0.4, 8.5]</t>
+          <t>3.3 [-0.3, 7.2]</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>-24.1 [-30.6, -18.6]</t>
+          <t>-26.5 [-31.6, -22.0]</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>-21.7 [-27.9, -16.1]</t>
+          <t>-23.9 [-28.9, -19.8]</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>1.04 [1.0, 1.07]</t>
+          <t>1.02 [1.0, 1.05]</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>0.44 [0.39, 0.47]</t>
+          <t>0.27 [0.23, 0.33]</t>
         </is>
       </c>
     </row>
@@ -1596,27 +1596,27 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>-22.3 [-28.1, -17.2]</t>
+          <t>-23.0 [-28.2, -17.8]</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>-49.3 [-57.6, -42.9]</t>
+          <t>-48.4 [-55.7, -42.2]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>-57.3 [-66.0, -50.2]</t>
+          <t>-58.0 [-65.3, -51.1]</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0.83 [0.78, 0.86]</t>
+          <t>0.84 [0.8, 0.87]</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>-0.34 [-0.35, -0.32]</t>
+          <t>-0.35 [-0.36, -0.33]</t>
         </is>
       </c>
     </row>
@@ -1631,27 +1631,27 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>4.6 [0.1, 9.1]</t>
+          <t>3.8 [-0.8, 8.1]</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>-24.5 [-30.4, -19.3]</t>
+          <t>-23.3 [-30.2, -17.3]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>-21.0 [-27.4, -14.8]</t>
+          <t>-20.1 [-26.7, -13.5]</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>1.04 [1.0, 1.07]</t>
+          <t>1.02 [1.0, 1.05]</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>0.08 [0.07, 0.08]</t>
+          <t>0.08 [0.07, 0.1]</t>
         </is>
       </c>
     </row>
@@ -1666,27 +1666,27 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17.9 [12.7, 23.9]</t>
+          <t>28.9 [21.8, 35.5]</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>-25.9 [-31.1, -21.2]</t>
+          <t>-26.9 [-31.6, -22.4]</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>-14.5 [-19.7, -9.6]</t>
+          <t>-7.4 [-13.4, -1.8]</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>1.15 [1.1, 1.19]</t>
+          <t>1.2 [1.16, 1.24]</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0.52 [0.45, 0.59]</t>
+          <t>0.79 [0.68, 0.88]</t>
         </is>
       </c>
     </row>
@@ -1701,27 +1701,27 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>38.3 [25.3, 61.7]</t>
+          <t>35.5 [26.7, 45.6]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>6.5 [0.4, 15.5]</t>
+          <t>13.6 [7.0, 19.6]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>52.6 [33.6, 79.9]</t>
+          <t>60.3 [46.9, 77.3]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>1.16 [1.12, 1.21]</t>
+          <t>1.19 [1.15, 1.23]</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2.27 [1.85, 2.71]</t>
+          <t>1.9 [1.52, 2.31]</t>
         </is>
       </c>
     </row>
@@ -1736,27 +1736,27 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>32.4 [23.8, 44.7]</t>
+          <t>29.0 [23.0, 36.7]</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2.7 [-4.7, 10.7]</t>
+          <t>4.5 [-1.5, 10.7]</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>38.2 [27.5, 53.3]</t>
+          <t>36.7 [28.0, 46.1]</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>1.14 [1.11, 1.19]</t>
+          <t>1.15 [1.12, 1.19]</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>1.14 [0.9, 1.31]</t>
+          <t>0.95 [0.83, 1.1]</t>
         </is>
       </c>
     </row>
@@ -1771,27 +1771,27 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>98.5 [74.6, 130.6]</t>
+          <t>68.2 [53.1, 90.8]</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>-49.9 [-63.2, -39.3]</t>
+          <t>-44.9 [-55.7, -37.0]</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>-23.5 [-35.1, -13.8]</t>
+          <t>-16.1 [-25.2, -8.4]</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>1.36 [1.29, 1.43]</t>
+          <t>1.26 [1.21, 1.32]</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>4.04 [3.38, 4.82]</t>
+          <t>2.49 [2.03, 3.28]</t>
         </is>
       </c>
     </row>
@@ -1806,27 +1806,27 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>7.4 [2.6, 12.6]</t>
+          <t>2.7 [-1.9, 7.8]</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>-24.0 [-29.5, -19.2]</t>
+          <t>-31.2 [-37.5, -25.7]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>-20.3 [-25.9, -14.9]</t>
+          <t>-29.7 [-36.2, -23.9]</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>1.05 [1.02, 1.08]</t>
+          <t>1.01 [0.99, 1.04]</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>0.24 [0.2, 0.27]</t>
+          <t>0.15 [0.14, 0.19]</t>
         </is>
       </c>
     </row>
@@ -1841,27 +1841,27 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>31.2 [25.2, 39.8]</t>
+          <t>39.6 [32.3, 48.1]</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>-12.5 [-17.9, -3.6]</t>
+          <t>-14.4 [-21.3, -5.8]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>13.4 [5.3, 33.1]</t>
+          <t>18.0 [6.1, 32.3]</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>1.18 [1.14, 1.22]</t>
+          <t>1.2 [1.17, 1.24]</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0.81 [0.75, 0.9]</t>
+          <t>0.85 [0.78, 0.92]</t>
         </is>
       </c>
     </row>
@@ -1876,27 +1876,27 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>6.4 [2.5, 10.8]</t>
+          <t>7.8 [4.2, 11.6]</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2.4 [-5.3, 9.8]</t>
+          <t>-3.9 [-9.3, 1.5]</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>8.6 [1.2, 17.8]</t>
+          <t>3.2 [-2.0, 9.2]</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>1.05 [1.02, 1.09]</t>
+          <t>1.05 [1.03, 1.08]</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>0.17 [0.06, 0.28]</t>
+          <t>0.21 [0.11, 0.31]</t>
         </is>
       </c>
     </row>
@@ -1911,27 +1911,27 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>13.2 [10.6, 16.5]</t>
+          <t>14.9 [11.6, 18.4]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>5.1 [1.4, 8.8]</t>
+          <t>5.8 [1.5, 10.9]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>19.1 [14.4, 24.9]</t>
+          <t>21.9 [16.3, 28.9]</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>1.11 [1.08, 1.14]</t>
+          <t>1.11 [1.09, 1.14]</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>0.53 [0.49, 0.56]</t>
+          <t>0.52 [0.49, 0.55]</t>
         </is>
       </c>
     </row>
@@ -1946,27 +1946,27 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>8.7 [4.5, 13.1]</t>
+          <t>14.8 [8.7, 20.5]</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>5.0 [-2.1, 12.5]</t>
+          <t>4.9 [-5.5, 14.3]</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>15.4 [8.4, 23.3]</t>
+          <t>23.4 [12.6, 33.8]</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>1.06 [1.03, 1.09]</t>
+          <t>1.05 [1.03, 1.08]</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>0.1 [0.09, 0.1]</t>
+          <t>0.11 [0.1, 0.13]</t>
         </is>
       </c>
     </row>
@@ -1981,27 +1981,27 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>14.0 [9.3, 21.0]</t>
+          <t>17.5 [12.4, 22.6]</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>-2.7 [-8.2, 2.0]</t>
+          <t>2.0 [-2.6, 7.2]</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>9.7 [3.5, 16.8]</t>
+          <t>19.4 [12.3, 27.3]</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>1.11 [1.07, 1.15]</t>
+          <t>1.09 [1.07, 1.12]</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>0.68 [0.62, 0.76]</t>
+          <t>0.64 [0.6, 0.69]</t>
         </is>
       </c>
     </row>

</xml_diff>